<commit_message>
lh ok faltan iamgenes
</commit_message>
<xml_diff>
--- a/plantillas/formatoLHSimple.xlsx
+++ b/plantillas/formatoLHSimple.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Gricardov.github.io\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED8244B-12F3-4171-AF30-7EDE0C039EAF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{503507C9-DEA3-4ABD-85A8-F9A334F270A9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="18" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -72,7 +73,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -106,16 +107,29 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <sz val="12"/>
+      <color rgb="FF248851"/>
+      <name val="Leelawadee"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Leelawadee"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF248851"/>
-      <name val="Calibri"/>
+      <color rgb="FF333F4F"/>
+      <name val="Leelawadee"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF333F4F"/>
+      <name val="Leelawadee"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -478,69 +492,69 @@
     <xf numFmtId="164" fontId="3" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Estilo 1" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -551,6 +565,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF333F4F"/>
       <color rgb="FF299B5D"/>
       <color rgb="FF248851"/>
       <color rgb="FF31A98A"/>
@@ -896,7 +911,7 @@
   <dimension ref="A1:BW1122"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="75" zoomScaleNormal="84" zoomScaleSheetLayoutView="106" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1149,7 +1164,7 @@
       <c r="BV3"/>
       <c r="BW3"/>
     </row>
-    <row r="4" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="20" t="s">
         <v>5</v>
@@ -1313,12 +1328,12 @@
     </row>
     <row r="6" spans="1:75" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
       <c r="H6"/>
       <c r="I6"/>
       <c r="J6"/>
@@ -1389,21 +1404,21 @@
       <c r="BW6"/>
     </row>
     <row r="7" spans="1:75" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="29"/>
-      <c r="B7" s="28" t="s">
+      <c r="A7" s="14"/>
+      <c r="B7" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14" t="s">
+      <c r="C7" s="36"/>
+      <c r="D7" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="37" t="s">
         <v>9</v>
       </c>
       <c r="H7"/>
@@ -1477,8 +1492,8 @@
     </row>
     <row r="8" spans="1:75" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
       <c r="D8" s="11"/>
       <c r="E8" s="12"/>
       <c r="F8" s="13"/>
@@ -1863,7 +1878,7 @@
     <row r="13" spans="1:75" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13"/>
-      <c r="C13" s="37"/>
+      <c r="C13" s="15"/>
       <c r="D13"/>
       <c r="E13"/>
       <c r="F13"/>

</xml_diff>